<commit_message>
ActiTime Automation Final Level
</commit_message>
<xml_diff>
--- a/ActiTime-Automation/Controller/data_Controller.xlsx
+++ b/ActiTime-Automation/Controller/data_Controller.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CurrentWorkSpace\DemoAutomationRepository\ActiTime-Automation\Controller\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9190"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -110,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,19 +123,13 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -300,9 +289,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -313,14 +303,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,137 +580,137 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="29">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4" ht="29">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" ht="29">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" ht="43.5">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:4" ht="43.5">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:4" ht="44" thickBot="1">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="13" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>